<commit_message>
updating looping and simonRPG files
</commit_message>
<xml_diff>
--- a/docs/simonRPG.xlsx
+++ b/docs/simonRPG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JURY-03\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E434EF95-FC52-4E20-A498-5A9C7439A19D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CF3397-C8BA-4734-AAD7-20BC77BD01D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" activeTab="1" xr2:uid="{CE87557A-F38C-4B0E-91DF-847348C0A2B3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{CE87557A-F38C-4B0E-91DF-847348C0A2B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -339,7 +339,28 @@
     <cellStyle name="20 % - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -652,8 +673,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,18 +884,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AD8A5C-AC34-4EFB-9D4F-46BB75576D03}">
-  <dimension ref="H6:AB22"/>
+  <dimension ref="G6:AB22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16:AB22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="4" style="14"/>
+    <col min="1" max="19" width="4" style="14"/>
+    <col min="20" max="20" width="4" style="14" customWidth="1"/>
+    <col min="21" max="16384" width="4" style="14"/>
   </cols>
   <sheetData>
-    <row r="6" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="7:28" x14ac:dyDescent="0.25">
       <c r="J6" s="14" t="s">
         <v>38</v>
       </c>
@@ -897,7 +920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="7:28" x14ac:dyDescent="0.25">
       <c r="I7" s="14" t="s">
         <v>38</v>
       </c>
@@ -926,7 +949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="7:28" x14ac:dyDescent="0.25">
       <c r="J8" s="14" t="s">
         <v>38</v>
       </c>
@@ -949,7 +972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="7:28" x14ac:dyDescent="0.25">
       <c r="J10" s="14" t="s">
         <v>38</v>
       </c>
@@ -984,7 +1007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="7:28" x14ac:dyDescent="0.25">
       <c r="I11" s="14" t="s">
         <v>38</v>
       </c>
@@ -1025,7 +1048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="7:28" x14ac:dyDescent="0.25">
       <c r="H12" s="14" t="s">
         <v>38</v>
       </c>
@@ -1072,7 +1095,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="7:28" x14ac:dyDescent="0.25">
       <c r="I13" s="14" t="s">
         <v>38</v>
       </c>
@@ -1113,7 +1136,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="7:28" x14ac:dyDescent="0.25">
       <c r="J14" s="14" t="s">
         <v>38</v>
       </c>
@@ -1148,227 +1171,421 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="7:28" x14ac:dyDescent="0.25">
+      <c r="G16" s="14">
+        <f>SQRT(V16)</f>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="H16" s="14">
+        <f t="shared" ref="H16:M16" si="0">SQRT(W16)</f>
+        <v>3.6055512754639891</v>
+      </c>
+      <c r="I16" s="14">
+        <f t="shared" si="0"/>
+        <v>3.1622776601683795</v>
+      </c>
+      <c r="J16" s="14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K16" s="14">
+        <f t="shared" si="0"/>
+        <v>3.1622776601683795</v>
+      </c>
+      <c r="L16" s="14">
+        <f t="shared" si="0"/>
+        <v>3.6055512754639891</v>
+      </c>
+      <c r="M16" s="14">
+        <f t="shared" si="0"/>
+        <v>4.2426406871192848</v>
+      </c>
       <c r="V16" s="14">
         <f>POWER(COLUMN()-COLUMN($Y$19),2) + POWER(ROW()-ROW($Y$19),2)</f>
         <v>18</v>
       </c>
       <c r="W16" s="14">
-        <f t="shared" ref="W16:AB22" si="0">POWER(COLUMN()-COLUMN($Y$19),2) + POWER(ROW()-ROW($Y$19),2)</f>
+        <f t="shared" ref="W16:AB22" si="1">POWER(COLUMN()-COLUMN($Y$19),2) + POWER(ROW()-ROW($Y$19),2)</f>
         <v>13</v>
       </c>
       <c r="X16" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="Y16" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="Z16" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="AA16" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="AB16" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="22:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:28" x14ac:dyDescent="0.25">
+      <c r="G17" s="14">
+        <f t="shared" ref="G17:G22" si="2">SQRT(V17)</f>
+        <v>3.6055512754639891</v>
+      </c>
+      <c r="H17" s="14">
+        <f t="shared" ref="H17:H22" si="3">SQRT(W17)</f>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="I17" s="14">
+        <f t="shared" ref="I17:I22" si="4">SQRT(X17)</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="J17" s="14">
+        <f t="shared" ref="J17:J22" si="5">SQRT(Y17)</f>
+        <v>2</v>
+      </c>
+      <c r="K17" s="14">
+        <f t="shared" ref="K17:K22" si="6">SQRT(Z17)</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="L17" s="14">
+        <f t="shared" ref="L17:L22" si="7">SQRT(AA17)</f>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="M17" s="14">
+        <f t="shared" ref="M17:M22" si="8">SQRT(AB17)</f>
+        <v>3.6055512754639891</v>
+      </c>
       <c r="V17" s="14">
-        <f t="shared" ref="V17:V22" si="1">POWER(COLUMN()-COLUMN($Y$19),2) + POWER(ROW()-ROW($Y$19),2)</f>
+        <f t="shared" ref="V17:V22" si="9">POWER(COLUMN()-COLUMN($Y$19),2) + POWER(ROW()-ROW($Y$19),2)</f>
         <v>13</v>
       </c>
       <c r="W17" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="X17" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Y17" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="Z17" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="AA17" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="AB17" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="22:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:28" x14ac:dyDescent="0.25">
+      <c r="G18" s="14">
+        <f t="shared" si="2"/>
+        <v>3.1622776601683795</v>
+      </c>
+      <c r="H18" s="14">
+        <f t="shared" si="3"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="I18" s="14">
+        <f t="shared" si="4"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="J18" s="14">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K18" s="14">
+        <f t="shared" si="6"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="L18" s="14">
+        <f t="shared" si="7"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="M18" s="14">
+        <f t="shared" si="8"/>
+        <v>3.1622776601683795</v>
+      </c>
       <c r="V18" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="W18" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="X18" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Y18" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Z18" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="AA18" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="AB18" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="22:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:28" x14ac:dyDescent="0.25">
+      <c r="G19" s="14">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="H19" s="14">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="I19" s="14">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J19" s="14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="14">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="L19" s="14">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="M19" s="14">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
       <c r="V19" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="W19" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="X19" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Y19" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z19" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AA19" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="AB19" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="22:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:28" x14ac:dyDescent="0.25">
+      <c r="G20" s="14">
+        <f t="shared" si="2"/>
+        <v>3.1622776601683795</v>
+      </c>
+      <c r="H20" s="14">
+        <f t="shared" si="3"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="I20" s="14">
+        <f t="shared" si="4"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="J20" s="14">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K20" s="14">
+        <f t="shared" si="6"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="L20" s="14">
+        <f t="shared" si="7"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="M20" s="14">
+        <f t="shared" si="8"/>
+        <v>3.1622776601683795</v>
+      </c>
       <c r="V20" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="W20" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="X20" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Y20" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Z20" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="AA20" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="AB20" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="22:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:28" x14ac:dyDescent="0.25">
+      <c r="G21" s="14">
+        <f t="shared" si="2"/>
+        <v>3.6055512754639891</v>
+      </c>
+      <c r="H21" s="14">
+        <f t="shared" si="3"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="I21" s="14">
+        <f t="shared" si="4"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="J21" s="14">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K21" s="14">
+        <f t="shared" si="6"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="L21" s="14">
+        <f t="shared" si="7"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="M21" s="14">
+        <f t="shared" si="8"/>
+        <v>3.6055512754639891</v>
+      </c>
       <c r="V21" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="W21" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="X21" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Y21" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="Z21" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="AA21" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="AB21" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="22:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:28" x14ac:dyDescent="0.25">
+      <c r="G22" s="14">
+        <f t="shared" si="2"/>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="H22" s="14">
+        <f t="shared" si="3"/>
+        <v>3.6055512754639891</v>
+      </c>
+      <c r="I22" s="14">
+        <f t="shared" si="4"/>
+        <v>3.1622776601683795</v>
+      </c>
+      <c r="J22" s="14">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="K22" s="14">
+        <f t="shared" si="6"/>
+        <v>3.1622776601683795</v>
+      </c>
+      <c r="L22" s="14">
+        <f t="shared" si="7"/>
+        <v>3.6055512754639891</v>
+      </c>
+      <c r="M22" s="14">
+        <f t="shared" si="8"/>
+        <v>4.2426406871192848</v>
+      </c>
       <c r="V22" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="W22" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="X22" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="Y22" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="Z22" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="AA22" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="AB22" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G16:M22">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>3.501</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="V16:AB22">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>12.26</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>